<commit_message>
p-Values and RBC updated
</commit_message>
<xml_diff>
--- a/RQ1/Data.xlsx
+++ b/RQ1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keshab\Documents\transfer-students-research\RQ1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{545EAB98-7044-41F0-BF70-EAA371FB9BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EAFBF1-0BE0-46E2-B2BF-A03FE0BE88B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="-250" windowWidth="12220" windowHeight="9600" xr2:uid="{D2A94699-4917-48B9-B250-C9D2500A0DC1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{D2A94699-4917-48B9-B250-C9D2500A0DC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Mean</t>
   </si>
@@ -69,13 +69,16 @@
   </si>
   <si>
     <t>CS2</t>
+  </si>
+  <si>
+    <t>RBC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +104,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +124,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -214,19 +229,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -250,11 +252,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -267,19 +269,32 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -290,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -298,9 +313,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -308,32 +320,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,110 +671,114 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="19"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>60</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>456</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>1.9166666666666601</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>1.9956140350877101</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>2</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>1.0133292447137201</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>0.99889084430459796</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>12942.5</v>
       </c>
-      <c r="K3" s="8">
-        <v>0.23633487989212501</v>
-      </c>
-      <c r="L3" s="1"/>
+      <c r="K3" s="23">
+        <v>0.47297</v>
+      </c>
+      <c r="L3" s="23">
+        <v>5.3911000000000001E-2</v>
+      </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3">
@@ -784,14 +808,16 @@
       <c r="J4" s="4">
         <v>6931</v>
       </c>
-      <c r="K4" s="4">
-        <v>3.0753659275935E-2</v>
-      </c>
-      <c r="L4" s="1"/>
+      <c r="K4" s="21">
+        <v>6.1603999999999999E-2</v>
+      </c>
+      <c r="L4" s="21">
+        <v>-0.16292300000000001</v>
+      </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3">
@@ -821,14 +847,17 @@
       <c r="J5" s="4">
         <v>2772.5</v>
       </c>
-      <c r="K5" s="5">
-        <v>2.0989574887203301E-8</v>
-      </c>
-      <c r="L5" s="1"/>
+      <c r="K5" s="22">
+        <v>4.226155E-8</v>
+      </c>
+      <c r="L5" s="20">
+        <v>-0.45466200000000001</v>
+      </c>
       <c r="M5" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>

</xml_diff>